<commit_message>
Fix admin chat status filtering and completion logic
- Fixed status filtering for '전체', '대기', '답변중', '완료' buttons
- Updated completion message detection logic to use correct messages
- Added proper status calculation for each user chat
- Fixed statistics calculation for pending, in-progress, and completed chats
- Improved representativeMessages logic with proper status assignment
- Enhanced filteredMessages to include status filtering
</commit_message>
<xml_diff>
--- a/수정사항.xlsx
+++ b/수정사항.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seoinjeong/Library/Mobile Documents/com~apple~CloudDocs/0. 프로젝트/ADMore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA60596-8040-8240-88AD-DC9ECE63977C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08388927-3B03-8B4B-B18D-61BC04DB4FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24540" yWindow="3360" windowWidth="24120" windowHeight="17380" xr2:uid="{812FD805-9A5A-E843-B914-C38D28068475}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -341,10 +341,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>관리자 1:1문의</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>오른쪽패널에 문의 경로 기능 추가시키기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -354,6 +350,18 @@
   </si>
   <si>
     <t>회원관리, 주문관리, 상품관리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:1문의</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">답변완료시 관리자와 유저의 채팅내용 저장/ 삭제 문제와 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저가 다시 채팅을 시작했을 때 유저의 상태와 관리자의 상태</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -961,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51ACB9AF-9FC2-C748-AD7B-775CDB889580}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1075,23 +1083,39 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
         <v>72</v>
       </c>
-      <c r="E20" t="s">
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
         <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="D24" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>